<commit_message>
added PDP & LIME
</commit_message>
<xml_diff>
--- a/data/Drilling_data.xlsx
+++ b/data/Drilling_data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28925"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Drilling_ISI_SummerProject\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4AF6AEF2-D55D-4160-85FC-693DD1C7F2D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E91EA52-6904-4201-A4B7-5A40B751A58D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{DE44A0B3-09BC-419E-A21B-AB6CFA0A6F3D}"/>
   </bookViews>
@@ -569,8 +569,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C828FC04-E47D-44B6-A006-CFE51F8FEBEE}">
   <dimension ref="A1:H166"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="77" workbookViewId="0">
-      <selection activeCell="Q13" sqref="Q13"/>
+    <sheetView tabSelected="1" topLeftCell="A134" zoomScale="77" workbookViewId="0">
+      <selection activeCell="H149" sqref="H149"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>